<commit_message>
Rearrange TS002 (remove temp data and console logs)
</commit_message>
<xml_diff>
--- a/TestCaseDocument.xlsx
+++ b/TestCaseDocument.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\InterviewAss\sonasu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\InterviewAss\sonasu\UIAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EEB704-863C-42A0-BDDD-FF7D1AA6B7BA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA22D512-C3B3-4A49-B815-C3B330B3EB7F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" tabRatio="649" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" tabRatio="649" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="409">
   <si>
     <t>Prerequisite</t>
   </si>
@@ -238,9 +238,6 @@
     <t>1. User account exists in system
 2. Application is accessible
 3. User is on login page</t>
-  </si>
-  <si>
-    <t>Active</t>
   </si>
   <si>
     <t>-</t>
@@ -2400,6 +2397,77 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="3" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="3" applyBorder="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="3" applyBorder="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="3" applyBorder="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2444,107 +2512,36 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="3" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="3" applyBorder="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="3" applyBorder="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="3" applyBorder="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2881,8 +2878,8 @@
   </sheetPr>
   <dimension ref="A1:AC24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2901,21 +2898,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
+      <c r="A3" s="93"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
     </row>
     <row r="4" spans="1:29" s="3" customFormat="1" ht="37.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -3052,7 +3049,7 @@
         <v>10</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G14" s="31" t="s">
         <v>46</v>
@@ -3072,16 +3069,16 @@
         <v>56</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I15" s="15"/>
     </row>
@@ -3093,7 +3090,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>30</v>
@@ -3102,10 +3099,10 @@
         <v>10</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I16" s="15"/>
     </row>
@@ -3117,7 +3114,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>30</v>
@@ -3126,10 +3123,10 @@
         <v>10</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="G17" s="118" t="s">
-        <v>405</v>
+        <v>283</v>
+      </c>
+      <c r="G17" s="91" t="s">
+        <v>404</v>
       </c>
       <c r="I17" s="15"/>
     </row>
@@ -3141,19 +3138,19 @@
         <v>28</v>
       </c>
       <c r="C18" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>407</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>408</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I18" s="15"/>
     </row>
@@ -3262,8 +3259,8 @@
   <dimension ref="A1:AI21"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <pane ySplit="8" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3287,10 +3284,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="75"/>
+      <c r="B1" s="98"/>
       <c r="C1" s="19" t="s">
         <v>25</v>
       </c>
@@ -3303,14 +3300,14 @@
       <c r="T1" s="26"/>
     </row>
     <row r="2" spans="1:34" ht="51.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="73" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="74"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="96" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="97"/>
       <c r="E2" s="19"/>
       <c r="O2" s="26"/>
       <c r="P2" s="26"/>
@@ -3320,10 +3317,10 @@
       <c r="T2" s="26"/>
     </row>
     <row r="3" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="72"/>
+      <c r="B3" s="95"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -3335,10 +3332,10 @@
       <c r="T3" s="26"/>
     </row>
     <row r="4" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="72"/>
+      <c r="B4" s="95"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -3351,10 +3348,10 @@
       <c r="T4" s="26"/>
     </row>
     <row r="5" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="72"/>
+      <c r="B5" s="95"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -3367,10 +3364,10 @@
       <c r="T5" s="26"/>
     </row>
     <row r="6" spans="1:34" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="72"/>
+      <c r="B6" s="95"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -3455,17 +3452,17 @@
         <v>59</v>
       </c>
       <c r="B9" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="D9" s="54" t="s">
         <v>92</v>
-      </c>
-      <c r="D9" s="54" t="s">
-        <v>93</v>
       </c>
       <c r="E9" s="52"/>
       <c r="F9" s="54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G9" s="52" t="s">
         <v>10</v>
@@ -3486,7 +3483,7 @@
     </row>
     <row r="10" spans="1:34" s="60" customFormat="1" ht="73" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="58" t="s">
         <v>61</v>
@@ -3495,7 +3492,7 @@
         <v>57</v>
       </c>
       <c r="D10" s="58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" s="58" t="s">
         <v>60</v>
@@ -3509,7 +3506,7 @@
       <c r="H10" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="58"/>
+      <c r="I10" s="52"/>
       <c r="J10" s="58"/>
       <c r="K10" s="58"/>
       <c r="L10" s="58"/>
@@ -3522,7 +3519,7 @@
     </row>
     <row r="11" spans="1:34" s="63" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A11" s="57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="62" t="s">
         <v>62</v>
@@ -3534,10 +3531,10 @@
         <v>64</v>
       </c>
       <c r="E11" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="62" t="s">
         <v>97</v>
-      </c>
-      <c r="F11" s="62" t="s">
-        <v>98</v>
       </c>
       <c r="G11" s="62" t="s">
         <v>10</v>
@@ -3545,7 +3542,7 @@
       <c r="H11" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="62"/>
+      <c r="I11" s="52"/>
       <c r="J11" s="62"/>
       <c r="K11" s="62"/>
       <c r="L11" s="58"/>
@@ -3558,22 +3555,22 @@
     </row>
     <row r="12" spans="1:34" s="63" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A12" s="57" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="64" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C12" s="64" t="s">
         <v>66</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F12" s="62" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G12" s="62" t="s">
         <v>10</v>
@@ -3581,12 +3578,10 @@
       <c r="H12" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="64" t="s">
-        <v>67</v>
-      </c>
+      <c r="I12" s="52"/>
       <c r="J12" s="64"/>
       <c r="K12" s="64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L12" s="58"/>
       <c r="M12" s="65"/>
@@ -3606,22 +3601,22 @@
     </row>
     <row r="13" spans="1:34" s="63" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B13" s="64" t="s">
         <v>65</v>
       </c>
       <c r="C13" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="E13" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="64" t="s">
-        <v>71</v>
-      </c>
       <c r="F13" s="62" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13" s="62" t="s">
         <v>41</v>
@@ -3629,12 +3624,10 @@
       <c r="H13" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="64" t="s">
-        <v>67</v>
-      </c>
+      <c r="I13" s="52"/>
       <c r="J13" s="64"/>
       <c r="K13" s="64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L13" s="58"/>
       <c r="M13" s="65"/>
@@ -3654,22 +3647,22 @@
     </row>
     <row r="14" spans="1:34" s="63" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="64" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="64" t="s">
+      <c r="E14" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="64" t="s">
-        <v>103</v>
-      </c>
       <c r="F14" s="62" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G14" s="62" t="s">
         <v>10</v>
@@ -3677,12 +3670,10 @@
       <c r="H14" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="64" t="s">
-        <v>67</v>
-      </c>
+      <c r="I14" s="52"/>
       <c r="J14" s="64"/>
       <c r="K14" s="64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L14" s="58"/>
       <c r="M14" s="65"/>
@@ -3702,22 +3693,22 @@
     </row>
     <row r="15" spans="1:34" s="63" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A15" s="57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="64" t="s">
         <v>104</v>
-      </c>
-      <c r="C15" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="64" t="s">
-        <v>105</v>
       </c>
       <c r="G15" s="62" t="s">
         <v>33</v>
@@ -3725,12 +3716,10 @@
       <c r="H15" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="64" t="s">
-        <v>67</v>
-      </c>
+      <c r="I15" s="52"/>
       <c r="J15" s="64"/>
       <c r="K15" s="64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L15" s="58"/>
       <c r="M15" s="65"/>
@@ -3750,20 +3739,20 @@
     </row>
     <row r="16" spans="1:34" s="63" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="64"/>
       <c r="D16" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="64" t="s">
+      <c r="F16" s="64" t="s">
         <v>107</v>
-      </c>
-      <c r="F16" s="64" t="s">
-        <v>108</v>
       </c>
       <c r="G16" s="62" t="s">
         <v>33</v>
@@ -3771,12 +3760,10 @@
       <c r="H16" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="64" t="s">
-        <v>67</v>
-      </c>
+      <c r="I16" s="52"/>
       <c r="J16" s="64"/>
       <c r="K16" s="64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L16" s="58"/>
       <c r="M16" s="65"/>
@@ -3796,22 +3783,22 @@
     </row>
     <row r="17" spans="1:26" s="63" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A17" s="57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="64" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="64" t="s">
         <v>76</v>
-      </c>
-      <c r="C17" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="64" t="s">
-        <v>77</v>
       </c>
       <c r="E17" s="58" t="s">
         <v>60</v>
       </c>
       <c r="F17" s="64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G17" s="62" t="s">
         <v>10</v>
@@ -3819,12 +3806,10 @@
       <c r="H17" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="64" t="s">
-        <v>67</v>
-      </c>
+      <c r="I17" s="52"/>
       <c r="J17" s="64"/>
       <c r="K17" s="64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L17" s="58"/>
       <c r="M17" s="65"/>
@@ -3844,22 +3829,22 @@
     </row>
     <row r="18" spans="1:26" s="66" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A18" s="57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" s="64" t="s">
-        <v>80</v>
-      </c>
       <c r="E18" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="64" t="s">
         <v>111</v>
-      </c>
-      <c r="F18" s="64" t="s">
-        <v>112</v>
       </c>
       <c r="G18" s="62" t="s">
         <v>10</v>
@@ -3867,12 +3852,10 @@
       <c r="H18" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="64" t="s">
-        <v>67</v>
-      </c>
+      <c r="I18" s="52"/>
       <c r="J18" s="64"/>
       <c r="K18" s="64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L18" s="58"/>
       <c r="M18" s="65"/>
@@ -3892,22 +3875,22 @@
     </row>
     <row r="19" spans="1:26" s="67" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B19" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="D19" s="64" t="s">
         <v>114</v>
-      </c>
-      <c r="D19" s="64" t="s">
-        <v>115</v>
       </c>
       <c r="E19" s="58" t="s">
         <v>60</v>
       </c>
       <c r="F19" s="65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G19" s="62" t="s">
         <v>10</v>
@@ -3915,6 +3898,7 @@
       <c r="H19" s="58" t="s">
         <v>31</v>
       </c>
+      <c r="I19" s="52"/>
       <c r="L19" s="58"/>
       <c r="O19" s="68"/>
       <c r="P19" s="68"/>
@@ -3925,22 +3909,22 @@
     </row>
     <row r="20" spans="1:26" s="69" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="64" t="s">
+      <c r="D20" s="65" t="s">
         <v>118</v>
-      </c>
-      <c r="D20" s="65" t="s">
-        <v>119</v>
       </c>
       <c r="E20" s="58" t="s">
         <v>60</v>
       </c>
       <c r="F20" s="64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G20" s="62" t="s">
         <v>10</v>
@@ -3948,6 +3932,7 @@
       <c r="H20" s="58" t="s">
         <v>30</v>
       </c>
+      <c r="I20" s="52"/>
       <c r="L20" s="58"/>
       <c r="O20" s="61"/>
       <c r="P20" s="61"/>
@@ -3975,7 +3960,7 @@
     <mergeCell ref="A5:B5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I10" xr:uid="{DDC46574-D4AC-4157-8C25-2E97C4ED56C2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I20" xr:uid="{DDC46574-D4AC-4157-8C25-2E97C4ED56C2}">
       <formula1>"Pass, Fail ,Not Executed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G20" xr:uid="{D5E07AC0-BBFD-4B5D-867A-E00A23F109AF}">
@@ -3994,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C57EAD-C42B-4BED-9CA2-3AD826B5B152}">
   <dimension ref="A1:AH27"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -4020,55 +4005,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="75"/>
+      <c r="B1" s="98"/>
       <c r="C1" s="30" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="50" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="79"/>
+      <c r="B2" s="102"/>
       <c r="C2" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="14" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="72"/>
+      <c r="B3" s="95"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:33" ht="14" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="72"/>
+      <c r="B4" s="95"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:33" ht="14" x14ac:dyDescent="0.3">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="72"/>
+      <c r="B5" s="95"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:33" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="72"/>
+      <c r="B6" s="95"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -4142,16 +4127,16 @@
         <v>43</v>
       </c>
       <c r="B9" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="E9" s="20" t="s">
         <v>126</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>127</v>
       </c>
       <c r="F9" s="20" t="s">
         <v>10</v>
@@ -4174,16 +4159,16 @@
         <v>44</v>
       </c>
       <c r="B10" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="D10" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="E10" s="28" t="s">
         <v>130</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>131</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>10</v>
@@ -4205,13 +4190,13 @@
         <v>45</v>
       </c>
       <c r="B11" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="E11" s="28" t="s">
         <v>133</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>134</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>33</v>
@@ -4233,13 +4218,13 @@
         <v>47</v>
       </c>
       <c r="B12" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="E12" s="28" t="s">
         <v>136</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>137</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>33</v>
@@ -4261,16 +4246,16 @@
         <v>48</v>
       </c>
       <c r="B13" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="D13" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="28" t="s">
         <v>139</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>140</v>
       </c>
       <c r="F13" s="20" t="s">
         <v>33</v>
@@ -4292,16 +4277,16 @@
         <v>49</v>
       </c>
       <c r="B14" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="D14" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="E14" s="28" t="s">
         <v>144</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>145</v>
       </c>
       <c r="F14" s="20" t="s">
         <v>33</v>
@@ -4323,16 +4308,16 @@
         <v>50</v>
       </c>
       <c r="B15" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="D15" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="E15" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>149</v>
       </c>
       <c r="F15" s="20" t="s">
         <v>33</v>
@@ -4351,16 +4336,16 @@
     </row>
     <row r="16" spans="1:33" s="28" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B16" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="E16" s="28" t="s">
         <v>151</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>152</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>33</v>
@@ -4379,16 +4364,16 @@
     </row>
     <row r="17" spans="1:20" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B17" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="E17" s="70" t="s">
         <v>154</v>
-      </c>
-      <c r="E17" s="88" t="s">
-        <v>155</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>33</v>
@@ -4407,19 +4392,19 @@
     </row>
     <row r="18" spans="1:20" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>156</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>157</v>
       </c>
       <c r="F18" s="20" t="s">
         <v>33</v>
@@ -4438,19 +4423,19 @@
     </row>
     <row r="19" spans="1:20" s="29" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B19" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="D19" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="E19" s="29" t="s">
         <v>160</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>161</v>
       </c>
       <c r="F19" s="20" t="s">
         <v>33</v>
@@ -4469,19 +4454,19 @@
     </row>
     <row r="20" spans="1:20" s="28" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B20" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="D20" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="E20" s="28" t="s">
         <v>166</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>167</v>
       </c>
       <c r="F20" s="20" t="s">
         <v>33</v>
@@ -4500,16 +4485,16 @@
     </row>
     <row r="21" spans="1:20" s="28" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B21" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="E21" s="28" t="s">
         <v>169</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>170</v>
       </c>
       <c r="F21" s="20" t="s">
         <v>33</v>
@@ -4528,19 +4513,19 @@
     </row>
     <row r="22" spans="1:20" s="28" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B22" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="C22" s="28" t="s">
-        <v>169</v>
-      </c>
       <c r="D22" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="28" t="s">
         <v>177</v>
-      </c>
-      <c r="E22" s="28" t="s">
-        <v>178</v>
       </c>
       <c r="F22" s="20" t="s">
         <v>33</v>
@@ -4559,19 +4544,19 @@
     </row>
     <row r="23" spans="1:20" s="28" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B23" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="D23" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E23" s="28" t="s">
         <v>180</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>181</v>
       </c>
       <c r="F23" s="20" t="s">
         <v>33</v>
@@ -4590,17 +4575,17 @@
     </row>
     <row r="24" spans="1:20" s="28" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B24" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="28" t="s">
         <v>182</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>183</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F24" s="20" t="s">
         <v>10</v>
@@ -4617,50 +4602,50 @@
       <c r="S24" s="44"/>
       <c r="T24" s="36"/>
     </row>
-    <row r="25" spans="1:20" s="98" customFormat="1" ht="175" x14ac:dyDescent="0.25">
-      <c r="A25" s="91" t="s">
-        <v>198</v>
-      </c>
-      <c r="B25" s="98" t="s">
+    <row r="25" spans="1:20" s="80" customFormat="1" ht="175" x14ac:dyDescent="0.25">
+      <c r="A25" s="73" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" s="80" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="80" t="s">
         <v>185</v>
       </c>
-      <c r="C25" s="98" t="s">
+      <c r="D25" s="73"/>
+      <c r="E25" s="80" t="s">
         <v>186</v>
       </c>
-      <c r="D25" s="91"/>
-      <c r="E25" s="98" t="s">
-        <v>187</v>
-      </c>
-      <c r="F25" s="92" t="s">
+      <c r="F25" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="92" t="s">
+      <c r="G25" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="M25" s="99"/>
+      <c r="M25" s="81"/>
       <c r="N25" s="44"/>
       <c r="O25" s="44"/>
       <c r="P25" s="44"/>
       <c r="Q25" s="44"/>
       <c r="R25" s="44"/>
       <c r="S25" s="44"/>
-      <c r="T25" s="100"/>
-    </row>
-    <row r="26" spans="1:20" s="96" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="93" t="s">
-        <v>199</v>
-      </c>
-      <c r="B26" s="97" t="s">
+      <c r="T25" s="82"/>
+    </row>
+    <row r="26" spans="1:20" s="78" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="75" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" s="79" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" s="83" t="s">
         <v>188</v>
       </c>
-      <c r="C26" s="101" t="s">
+      <c r="D26" s="78" t="s">
         <v>189</v>
       </c>
-      <c r="D26" s="96" t="s">
+      <c r="E26" s="83" t="s">
         <v>190</v>
-      </c>
-      <c r="E26" s="101" t="s">
-        <v>191</v>
       </c>
       <c r="F26" s="20" t="s">
         <v>10</v>
@@ -4669,18 +4654,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="96" customFormat="1" ht="88" x14ac:dyDescent="0.3">
-      <c r="A27" s="93" t="s">
-        <v>200</v>
-      </c>
-      <c r="B27" s="94" t="s">
+    <row r="27" spans="1:20" s="78" customFormat="1" ht="88" x14ac:dyDescent="0.3">
+      <c r="A27" s="75" t="s">
+        <v>199</v>
+      </c>
+      <c r="B27" s="76" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" s="77" t="s">
         <v>192</v>
       </c>
-      <c r="C27" s="95" t="s">
+      <c r="E27" s="79" t="s">
         <v>193</v>
-      </c>
-      <c r="E27" s="97" t="s">
-        <v>194</v>
       </c>
       <c r="F27" s="20" t="s">
         <v>10</v>
@@ -4719,7 +4704,7 @@
   <dimension ref="A1:AI27"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9:XFD27"/>
     </sheetView>
   </sheetViews>
@@ -4744,62 +4729,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="80" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="81"/>
+      <c r="D1" s="104"/>
     </row>
     <row r="2" spans="1:34" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="73" t="s">
-        <v>202</v>
-      </c>
-      <c r="D2" s="74"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" s="97"/>
     </row>
     <row r="3" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="83"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="83"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="106"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="83"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="106"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:34" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="85"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="108"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="O6" s="41"/>
@@ -4814,7 +4799,7 @@
       <c r="A8" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="80" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="46" t="s">
@@ -4870,21 +4855,21 @@
       <c r="AG8" s="13"/>
       <c r="AH8" s="13"/>
     </row>
-    <row r="9" spans="1:34" s="93" customFormat="1" ht="100" x14ac:dyDescent="0.25">
-      <c r="A9" s="93" t="s">
+    <row r="9" spans="1:34" s="75" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="A9" s="75" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="75" t="s">
         <v>210</v>
       </c>
-      <c r="B9" s="93" t="s">
+      <c r="C9" s="75" t="s">
         <v>211</v>
       </c>
-      <c r="C9" s="93" t="s">
+      <c r="D9" s="75" t="s">
         <v>212</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="F9" s="75" t="s">
         <v>213</v>
-      </c>
-      <c r="F9" s="93" t="s">
-        <v>214</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>41</v>
@@ -4893,21 +4878,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:34" s="93" customFormat="1" ht="100" x14ac:dyDescent="0.25">
-      <c r="A10" s="93" t="s">
-        <v>203</v>
-      </c>
-      <c r="B10" s="93" t="s">
+    <row r="10" spans="1:34" s="75" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="A10" s="75" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="75" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="75" t="s">
         <v>215</v>
       </c>
-      <c r="C10" s="93" t="s">
+      <c r="D10" s="75" t="s">
         <v>216</v>
       </c>
-      <c r="D10" s="93" t="s">
+      <c r="F10" s="77" t="s">
         <v>217</v>
-      </c>
-      <c r="F10" s="95" t="s">
-        <v>218</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>41</v>
@@ -4916,18 +4901,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:34" s="119" customFormat="1" ht="100" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="s">
-        <v>204</v>
-      </c>
-      <c r="B11" s="119" t="s">
+    <row r="11" spans="1:34" s="92" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="A11" s="75" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" s="92" t="s">
+        <v>218</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="F11" s="92" t="s">
         <v>220</v>
-      </c>
-      <c r="F11" s="119" t="s">
-        <v>221</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>41</v>
@@ -4936,21 +4921,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:34" s="119" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="93" t="s">
-        <v>205</v>
-      </c>
-      <c r="B12" s="119" t="s">
+    <row r="12" spans="1:34" s="92" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="75" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="92" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="92" t="s">
         <v>222</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="D12" s="92" t="s">
         <v>223</v>
       </c>
-      <c r="D12" s="119" t="s">
+      <c r="F12" s="92" t="s">
         <v>224</v>
-      </c>
-      <c r="F12" s="119" t="s">
-        <v>225</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>41</v>
@@ -4959,18 +4944,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:34" s="119" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="93" t="s">
-        <v>206</v>
-      </c>
-      <c r="B13" s="119" t="s">
+    <row r="13" spans="1:34" s="92" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="75" t="s">
+        <v>205</v>
+      </c>
+      <c r="B13" s="92" t="s">
+        <v>225</v>
+      </c>
+      <c r="D13" s="92" t="s">
         <v>226</v>
       </c>
-      <c r="D13" s="119" t="s">
+      <c r="F13" s="92" t="s">
         <v>227</v>
-      </c>
-      <c r="F13" s="119" t="s">
-        <v>228</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>41</v>
@@ -4979,18 +4964,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:34" s="119" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="93" t="s">
-        <v>207</v>
-      </c>
-      <c r="B14" s="119" t="s">
+    <row r="14" spans="1:34" s="92" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="75" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="92" t="s">
+        <v>228</v>
+      </c>
+      <c r="D14" s="92" t="s">
         <v>229</v>
       </c>
-      <c r="D14" s="119" t="s">
+      <c r="F14" s="92" t="s">
         <v>230</v>
-      </c>
-      <c r="F14" s="119" t="s">
-        <v>231</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>41</v>
@@ -4999,19 +4984,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:34" s="119" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="93" t="s">
-        <v>208</v>
-      </c>
-      <c r="B15" s="119" t="s">
+    <row r="15" spans="1:34" s="92" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="75" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="92" t="s">
+        <v>231</v>
+      </c>
+      <c r="D15" s="92" t="s">
         <v>232</v>
       </c>
-      <c r="D15" s="119" t="s">
+      <c r="E15" s="75"/>
+      <c r="F15" s="92" t="s">
         <v>233</v>
-      </c>
-      <c r="E15" s="93"/>
-      <c r="F15" s="119" t="s">
-        <v>234</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>41</v>
@@ -5020,19 +5005,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:34" s="119" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="93" t="s">
-        <v>209</v>
-      </c>
-      <c r="B16" s="119" t="s">
+    <row r="16" spans="1:34" s="92" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="75" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="92" t="s">
+        <v>234</v>
+      </c>
+      <c r="D16" s="92" t="s">
         <v>235</v>
       </c>
-      <c r="D16" s="119" t="s">
+      <c r="E16" s="75"/>
+      <c r="F16" s="92" t="s">
         <v>236</v>
-      </c>
-      <c r="E16" s="93"/>
-      <c r="F16" s="119" t="s">
-        <v>237</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>41</v>
@@ -5041,18 +5026,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="96" customFormat="1" ht="100" x14ac:dyDescent="0.25">
-      <c r="A17" s="93" t="s">
-        <v>271</v>
-      </c>
-      <c r="B17" s="97" t="s">
+    <row r="17" spans="1:8" s="78" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="A17" s="75" t="s">
+        <v>270</v>
+      </c>
+      <c r="B17" s="79" t="s">
+        <v>237</v>
+      </c>
+      <c r="D17" s="77" t="s">
         <v>238</v>
       </c>
-      <c r="D17" s="95" t="s">
+      <c r="F17" s="77" t="s">
         <v>239</v>
-      </c>
-      <c r="F17" s="95" t="s">
-        <v>240</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>41</v>
@@ -5061,168 +5046,168 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="96" customFormat="1" ht="100" x14ac:dyDescent="0.25">
-      <c r="A18" s="93" t="s">
-        <v>272</v>
-      </c>
-      <c r="B18" s="97" t="s">
+    <row r="18" spans="1:8" s="78" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="A18" s="75" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="79" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" s="77" t="s">
         <v>241</v>
       </c>
-      <c r="D18" s="95" t="s">
+      <c r="F18" s="79" t="s">
         <v>242</v>
-      </c>
-      <c r="F18" s="97" t="s">
-        <v>243</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="96" customFormat="1" ht="100" x14ac:dyDescent="0.25">
-      <c r="A19" s="93" t="s">
-        <v>273</v>
-      </c>
-      <c r="B19" s="97" t="s">
+    <row r="19" spans="1:8" s="78" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="A19" s="75" t="s">
+        <v>272</v>
+      </c>
+      <c r="B19" s="79" t="s">
+        <v>243</v>
+      </c>
+      <c r="D19" s="77" t="s">
         <v>244</v>
       </c>
-      <c r="D19" s="95" t="s">
+      <c r="F19" s="79" t="s">
         <v>245</v>
-      </c>
-      <c r="F19" s="97" t="s">
-        <v>246</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="96" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="93" t="s">
-        <v>274</v>
-      </c>
-      <c r="B20" s="97" t="s">
+    <row r="20" spans="1:8" s="78" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="75" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20" s="79" t="s">
+        <v>246</v>
+      </c>
+      <c r="D20" s="77" t="s">
         <v>247</v>
       </c>
-      <c r="D20" s="95" t="s">
+      <c r="F20" s="79" t="s">
         <v>248</v>
-      </c>
-      <c r="F20" s="97" t="s">
-        <v>249</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="96" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="93" t="s">
-        <v>275</v>
-      </c>
-      <c r="B21" s="97" t="s">
+    <row r="21" spans="1:8" s="78" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="75" t="s">
+        <v>274</v>
+      </c>
+      <c r="B21" s="79" t="s">
+        <v>249</v>
+      </c>
+      <c r="D21" s="77" t="s">
         <v>250</v>
       </c>
-      <c r="D21" s="95" t="s">
+      <c r="F21" s="79" t="s">
         <v>251</v>
-      </c>
-      <c r="F21" s="97" t="s">
-        <v>252</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="96" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="93" t="s">
-        <v>276</v>
-      </c>
-      <c r="B22" s="97" t="s">
+    <row r="22" spans="1:8" s="78" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="75" t="s">
+        <v>275</v>
+      </c>
+      <c r="B22" s="79" t="s">
+        <v>252</v>
+      </c>
+      <c r="D22" s="77" t="s">
         <v>253</v>
       </c>
-      <c r="D22" s="95" t="s">
+      <c r="F22" s="79" t="s">
         <v>254</v>
-      </c>
-      <c r="F22" s="97" t="s">
-        <v>255</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="96" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="93" t="s">
-        <v>277</v>
-      </c>
-      <c r="B23" s="97" t="s">
+    <row r="23" spans="1:8" s="78" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="75" t="s">
+        <v>276</v>
+      </c>
+      <c r="B23" s="79" t="s">
+        <v>255</v>
+      </c>
+      <c r="D23" s="77" t="s">
         <v>256</v>
       </c>
-      <c r="D23" s="95" t="s">
+      <c r="F23" s="79" t="s">
         <v>257</v>
-      </c>
-      <c r="F23" s="97" t="s">
-        <v>258</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="96" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="93" t="s">
-        <v>278</v>
-      </c>
-      <c r="B24" s="97" t="s">
+    <row r="24" spans="1:8" s="78" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="75" t="s">
+        <v>277</v>
+      </c>
+      <c r="B24" s="79" t="s">
+        <v>258</v>
+      </c>
+      <c r="D24" s="77" t="s">
         <v>259</v>
       </c>
-      <c r="D24" s="95" t="s">
+      <c r="F24" s="79" t="s">
         <v>260</v>
-      </c>
-      <c r="F24" s="97" t="s">
-        <v>261</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="96" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="93" t="s">
-        <v>279</v>
-      </c>
-      <c r="B25" s="97" t="s">
+    <row r="25" spans="1:8" s="78" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="75" t="s">
+        <v>278</v>
+      </c>
+      <c r="B25" s="79" t="s">
+        <v>261</v>
+      </c>
+      <c r="D25" s="77" t="s">
         <v>262</v>
       </c>
-      <c r="D25" s="95" t="s">
+      <c r="F25" s="79" t="s">
         <v>263</v>
-      </c>
-      <c r="F25" s="97" t="s">
-        <v>264</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="96" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="93" t="s">
+    <row r="26" spans="1:8" s="78" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="75" t="s">
+        <v>279</v>
+      </c>
+      <c r="B26" s="79" t="s">
+        <v>264</v>
+      </c>
+      <c r="D26" s="77" t="s">
+        <v>265</v>
+      </c>
+      <c r="F26" s="77" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="78" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="75" t="s">
         <v>280</v>
       </c>
-      <c r="B26" s="97" t="s">
-        <v>265</v>
-      </c>
-      <c r="D26" s="95" t="s">
-        <v>266</v>
-      </c>
-      <c r="F26" s="95" t="s">
+      <c r="B27" s="79" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" s="96" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="93" t="s">
-        <v>281</v>
-      </c>
-      <c r="B27" s="97" t="s">
+      <c r="D27" s="77" t="s">
         <v>268</v>
       </c>
-      <c r="D27" s="95" t="s">
+      <c r="F27" s="79" t="s">
         <v>269</v>
-      </c>
-      <c r="F27" s="97" t="s">
-        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -5264,94 +5249,94 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.36328125" style="90" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" style="90" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" style="90" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" style="90" customWidth="1"/>
-    <col min="6" max="6" width="23" style="90" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" style="90" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" style="90" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" style="90" customWidth="1"/>
-    <col min="10" max="11" width="20.54296875" style="90" customWidth="1"/>
-    <col min="12" max="12" width="17.90625" style="90" customWidth="1"/>
-    <col min="13" max="14" width="0" style="90" hidden="1" customWidth="1"/>
-    <col min="15" max="18" width="8.90625" style="102" customWidth="1"/>
-    <col min="19" max="19" width="0" style="102" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="8.90625" style="102" customWidth="1"/>
-    <col min="21" max="35" width="0" style="90" hidden="1" customWidth="1"/>
-    <col min="36" max="16384" width="8.90625" style="90" hidden="1"/>
+    <col min="1" max="2" width="17.36328125" style="72" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" style="72" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" style="72" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" style="72" customWidth="1"/>
+    <col min="6" max="6" width="23" style="72" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" style="72" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" style="72" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" style="72" customWidth="1"/>
+    <col min="10" max="11" width="20.54296875" style="72" customWidth="1"/>
+    <col min="12" max="12" width="17.90625" style="72" customWidth="1"/>
+    <col min="13" max="14" width="0" style="72" hidden="1" customWidth="1"/>
+    <col min="15" max="18" width="8.90625" style="84" customWidth="1"/>
+    <col min="19" max="19" width="0" style="84" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="8.90625" style="84" customWidth="1"/>
+    <col min="21" max="35" width="0" style="72" hidden="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.90625" style="72" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="109" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="104" t="s">
+      <c r="B1" s="109"/>
+      <c r="C1" s="110" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="105"/>
+      <c r="D1" s="111"/>
     </row>
     <row r="2" spans="1:34" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="73" t="s">
-        <v>287</v>
-      </c>
-      <c r="D2" s="74"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="96" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" s="97"/>
     </row>
     <row r="3" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="109"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="83"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A4" s="108" t="s">
+      <c r="A4" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="83"/>
+      <c r="B4" s="115"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="106"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A5" s="108" t="s">
+      <c r="A5" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="109"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="83"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="106"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
     </row>
-    <row r="6" spans="1:34" s="112" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A6" s="108" t="s">
+    <row r="6" spans="1:34" s="85" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="A6" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="110"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
+      <c r="B6" s="116"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
-      <c r="O6" s="113"/>
-      <c r="P6" s="113"/>
-      <c r="Q6" s="113"/>
-      <c r="R6" s="113"/>
-      <c r="S6" s="113"/>
-      <c r="T6" s="113"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="86"/>
+      <c r="Q6" s="86"/>
+      <c r="R6" s="86"/>
+      <c r="S6" s="86"/>
+      <c r="T6" s="86"/>
     </row>
     <row r="7" spans="1:34" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="114"/>
-    </row>
-    <row r="8" spans="1:34" s="117" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="87"/>
+    </row>
+    <row r="8" spans="1:34" s="90" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>36</v>
       </c>
@@ -5390,9 +5375,9 @@
       </c>
       <c r="M8" s="23"/>
       <c r="N8" s="19"/>
-      <c r="O8" s="115"/>
-      <c r="P8" s="115"/>
-      <c r="Q8" s="115"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="88"/>
       <c r="R8" s="43"/>
       <c r="S8" s="43"/>
       <c r="T8" s="43"/>
@@ -5408,24 +5393,24 @@
       <c r="AD8" s="24"/>
       <c r="AE8" s="24"/>
       <c r="AF8" s="24"/>
-      <c r="AG8" s="116"/>
-      <c r="AH8" s="116"/>
-    </row>
-    <row r="9" spans="1:34" s="101" customFormat="1" ht="187.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="95" t="s">
-        <v>286</v>
-      </c>
-      <c r="B9" s="95" t="s">
+      <c r="AG8" s="89"/>
+      <c r="AH8" s="89"/>
+    </row>
+    <row r="9" spans="1:34" s="83" customFormat="1" ht="187.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="77" t="s">
         <v>285</v>
       </c>
-      <c r="C9" s="95" t="s">
-        <v>212</v>
-      </c>
-      <c r="D9" s="95" t="s">
+      <c r="B9" s="77" t="s">
+        <v>284</v>
+      </c>
+      <c r="C9" s="77" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" s="77" t="s">
+        <v>287</v>
+      </c>
+      <c r="F9" s="77" t="s">
         <v>288</v>
-      </c>
-      <c r="F9" s="95" t="s">
-        <v>289</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>33</v>
@@ -5434,309 +5419,309 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:34" s="101" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="95" t="s">
+    <row r="10" spans="1:34" s="83" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="77" t="s">
+        <v>350</v>
+      </c>
+      <c r="B10" s="77" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" s="77" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>290</v>
+      </c>
+      <c r="F10" s="77" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" s="83" customFormat="1" ht="175" x14ac:dyDescent="0.25">
+      <c r="A11" s="77" t="s">
         <v>351</v>
       </c>
-      <c r="B10" s="95" t="s">
-        <v>290</v>
-      </c>
-      <c r="C10" s="95" t="s">
-        <v>216</v>
-      </c>
-      <c r="D10" s="95" t="s">
-        <v>291</v>
-      </c>
-      <c r="F10" s="95" t="s">
+      <c r="B11" s="77" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="11" spans="1:34" s="101" customFormat="1" ht="175" x14ac:dyDescent="0.25">
-      <c r="A11" s="95" t="s">
+      <c r="D11" s="77" t="s">
+        <v>293</v>
+      </c>
+      <c r="F11" s="77" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" s="83" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="77" t="s">
         <v>352</v>
       </c>
-      <c r="B11" s="95" t="s">
-        <v>293</v>
-      </c>
-      <c r="D11" s="95" t="s">
-        <v>294</v>
-      </c>
-      <c r="F11" s="95" t="s">
+      <c r="B12" s="77" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="12" spans="1:34" s="101" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="95" t="s">
+      <c r="D12" s="77" t="s">
+        <v>296</v>
+      </c>
+      <c r="F12" s="77" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" s="83" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="77" t="s">
         <v>353</v>
       </c>
-      <c r="B12" s="95" t="s">
-        <v>296</v>
-      </c>
-      <c r="D12" s="95" t="s">
-        <v>297</v>
-      </c>
-      <c r="F12" s="95" t="s">
+      <c r="B13" s="77" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="13" spans="1:34" s="101" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="95" t="s">
+      <c r="D13" s="77" t="s">
+        <v>299</v>
+      </c>
+      <c r="E13" s="77" t="s">
+        <v>300</v>
+      </c>
+      <c r="F13" s="77" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" s="83" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="77" t="s">
         <v>354</v>
       </c>
-      <c r="B13" s="95" t="s">
-        <v>299</v>
-      </c>
-      <c r="D13" s="95" t="s">
-        <v>300</v>
-      </c>
-      <c r="E13" s="95" t="s">
-        <v>301</v>
-      </c>
-      <c r="F13" s="95" t="s">
+      <c r="B14" s="77" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" s="101" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="95" t="s">
+      <c r="D14" s="77" t="s">
+        <v>303</v>
+      </c>
+      <c r="E14" s="77" t="s">
+        <v>304</v>
+      </c>
+      <c r="F14" s="77" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" s="83" customFormat="1" ht="250" x14ac:dyDescent="0.25">
+      <c r="A15" s="77" t="s">
         <v>355</v>
       </c>
-      <c r="B14" s="95" t="s">
-        <v>303</v>
-      </c>
-      <c r="D14" s="95" t="s">
-        <v>304</v>
-      </c>
-      <c r="E14" s="95" t="s">
-        <v>305</v>
-      </c>
-      <c r="F14" s="95" t="s">
+      <c r="B15" s="77" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="15" spans="1:34" s="101" customFormat="1" ht="250" x14ac:dyDescent="0.25">
-      <c r="A15" s="95" t="s">
+      <c r="D15" s="77" t="s">
+        <v>307</v>
+      </c>
+      <c r="F15" s="77" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" s="83" customFormat="1" ht="125" x14ac:dyDescent="0.25">
+      <c r="A16" s="77" t="s">
         <v>356</v>
       </c>
-      <c r="B15" s="95" t="s">
-        <v>307</v>
-      </c>
-      <c r="D15" s="95" t="s">
-        <v>308</v>
-      </c>
-      <c r="F15" s="95" t="s">
+      <c r="B16" s="77" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="16" spans="1:34" s="101" customFormat="1" ht="125" x14ac:dyDescent="0.25">
-      <c r="A16" s="95" t="s">
+      <c r="D16" s="77" t="s">
+        <v>310</v>
+      </c>
+      <c r="F16" s="77" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="83" customFormat="1" ht="175" x14ac:dyDescent="0.25">
+      <c r="A17" s="77" t="s">
         <v>357</v>
       </c>
-      <c r="B16" s="95" t="s">
-        <v>310</v>
-      </c>
-      <c r="D16" s="95" t="s">
-        <v>311</v>
-      </c>
-      <c r="F16" s="95" t="s">
+      <c r="B17" s="77" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" s="101" customFormat="1" ht="175" x14ac:dyDescent="0.25">
-      <c r="A17" s="95" t="s">
+      <c r="D17" s="77" t="s">
+        <v>313</v>
+      </c>
+      <c r="F17" s="77" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="83" customFormat="1" ht="137.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="77" t="s">
         <v>358</v>
       </c>
-      <c r="B17" s="95" t="s">
-        <v>313</v>
-      </c>
-      <c r="D17" s="95" t="s">
-        <v>314</v>
-      </c>
-      <c r="F17" s="95" t="s">
+      <c r="B18" s="77" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" s="101" customFormat="1" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="95" t="s">
+      <c r="D18" s="77" t="s">
+        <v>316</v>
+      </c>
+      <c r="F18" s="77" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="83" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="77" t="s">
         <v>359</v>
       </c>
-      <c r="B18" s="95" t="s">
-        <v>316</v>
-      </c>
-      <c r="D18" s="95" t="s">
-        <v>317</v>
-      </c>
-      <c r="F18" s="95" t="s">
+      <c r="B19" s="77" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" s="101" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="95" t="s">
+      <c r="D19" s="77" t="s">
+        <v>319</v>
+      </c>
+      <c r="F19" s="77" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="83" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A20" s="77" t="s">
         <v>360</v>
       </c>
-      <c r="B19" s="95" t="s">
-        <v>319</v>
-      </c>
-      <c r="D19" s="95" t="s">
-        <v>320</v>
-      </c>
-      <c r="F19" s="95" t="s">
+      <c r="B20" s="77" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" s="101" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A20" s="95" t="s">
+      <c r="D20" s="77" t="s">
+        <v>322</v>
+      </c>
+      <c r="F20" s="77" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="83" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A21" s="77" t="s">
         <v>361</v>
       </c>
-      <c r="B20" s="95" t="s">
-        <v>322</v>
-      </c>
-      <c r="D20" s="95" t="s">
-        <v>323</v>
-      </c>
-      <c r="F20" s="95" t="s">
+      <c r="B21" s="77" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" s="101" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A21" s="95" t="s">
+      <c r="D21" s="77" t="s">
+        <v>325</v>
+      </c>
+      <c r="E21" s="77" t="s">
+        <v>326</v>
+      </c>
+      <c r="F21" s="77" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="83" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="77" t="s">
         <v>362</v>
       </c>
-      <c r="B21" s="95" t="s">
-        <v>325</v>
-      </c>
-      <c r="D21" s="95" t="s">
-        <v>326</v>
-      </c>
-      <c r="E21" s="95" t="s">
-        <v>327</v>
-      </c>
-      <c r="F21" s="95" t="s">
+      <c r="B22" s="77" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" s="101" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="95" t="s">
+      <c r="D22" s="77" t="s">
+        <v>329</v>
+      </c>
+      <c r="E22" s="77" t="s">
+        <v>330</v>
+      </c>
+      <c r="F22" s="77" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="83" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="77" t="s">
         <v>363</v>
       </c>
-      <c r="B22" s="95" t="s">
-        <v>329</v>
-      </c>
-      <c r="D22" s="95" t="s">
-        <v>330</v>
-      </c>
-      <c r="E22" s="95" t="s">
-        <v>331</v>
-      </c>
-      <c r="F22" s="95" t="s">
+      <c r="B23" s="77" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" s="101" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="95" t="s">
+      <c r="D23" s="77" t="s">
+        <v>333</v>
+      </c>
+      <c r="F23" s="77" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="83" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="77" t="s">
         <v>364</v>
       </c>
-      <c r="B23" s="95" t="s">
-        <v>333</v>
-      </c>
-      <c r="D23" s="95" t="s">
-        <v>334</v>
-      </c>
-      <c r="F23" s="95" t="s">
+      <c r="B24" s="77" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" s="101" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="95" t="s">
+      <c r="D24" s="77" t="s">
+        <v>336</v>
+      </c>
+      <c r="F24" s="77" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="83" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="77" t="s">
         <v>365</v>
       </c>
-      <c r="B24" s="95" t="s">
-        <v>336</v>
-      </c>
-      <c r="D24" s="95" t="s">
-        <v>337</v>
-      </c>
-      <c r="F24" s="95" t="s">
+      <c r="B25" s="77" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" s="101" customFormat="1" ht="162.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="95" t="s">
+      <c r="D25" s="77" t="s">
+        <v>339</v>
+      </c>
+      <c r="F25" s="77" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="83" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A26" s="77" t="s">
         <v>366</v>
       </c>
-      <c r="B25" s="95" t="s">
-        <v>339</v>
-      </c>
-      <c r="D25" s="95" t="s">
-        <v>340</v>
-      </c>
-      <c r="F25" s="95" t="s">
+      <c r="B26" s="77" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" s="101" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A26" s="95" t="s">
+      <c r="D26" s="77" t="s">
+        <v>342</v>
+      </c>
+      <c r="F26" s="77" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="83" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A27" s="77" t="s">
+        <v>384</v>
+      </c>
+      <c r="B27" s="77" t="s">
+        <v>344</v>
+      </c>
+      <c r="D27" s="77" t="s">
+        <v>345</v>
+      </c>
+      <c r="F27" s="77" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="83" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A28" s="77" t="s">
         <v>367</v>
       </c>
-      <c r="B26" s="95" t="s">
-        <v>342</v>
-      </c>
-      <c r="D26" s="95" t="s">
-        <v>343</v>
-      </c>
-      <c r="F26" s="95" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="101" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A27" s="95" t="s">
+      <c r="B28" s="77" t="s">
+        <v>347</v>
+      </c>
+      <c r="D28" s="77" t="s">
+        <v>348</v>
+      </c>
+      <c r="F28" s="77" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="83" customFormat="1" ht="50" x14ac:dyDescent="0.25">
+      <c r="A29" s="77" t="s">
+        <v>408</v>
+      </c>
+      <c r="B29" s="77" t="s">
         <v>385</v>
-      </c>
-      <c r="B27" s="95" t="s">
-        <v>345</v>
-      </c>
-      <c r="D27" s="95" t="s">
-        <v>346</v>
-      </c>
-      <c r="F27" s="95" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="101" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A28" s="95" t="s">
-        <v>368</v>
-      </c>
-      <c r="B28" s="95" t="s">
-        <v>348</v>
-      </c>
-      <c r="D28" s="95" t="s">
-        <v>349</v>
-      </c>
-      <c r="F28" s="95" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="101" customFormat="1" ht="50" x14ac:dyDescent="0.25">
-      <c r="A29" s="95" t="s">
-        <v>409</v>
-      </c>
-      <c r="B29" s="95" t="s">
-        <v>386</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9" xr:uid="{405F6E85-09AD-402F-B890-DCD9B135CAA9}">
@@ -5755,7 +5740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB623CDC-C814-4ACB-B94D-7503908CABD8}">
   <dimension ref="A1:AI16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
@@ -5781,60 +5766,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="80" t="s">
+      <c r="B1" s="98"/>
+      <c r="C1" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="81"/>
+      <c r="D1" s="104"/>
     </row>
     <row r="2" spans="1:34" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="74"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="97"/>
     </row>
     <row r="3" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="83"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="106"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="83"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="106"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:34" ht="14" x14ac:dyDescent="0.3">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="83"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="106"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:34" s="18" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="86"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="O6" s="41"/>
@@ -5909,16 +5894,16 @@
     </row>
     <row r="9" spans="1:34" s="28" customFormat="1" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B9" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="D9" s="28" t="s">
         <v>369</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="F9" s="28" t="s">
         <v>370</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>371</v>
       </c>
       <c r="H9" s="20"/>
       <c r="N9" s="33"/>
@@ -5932,16 +5917,16 @@
     </row>
     <row r="10" spans="1:34" s="28" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B10" s="28" t="s">
+        <v>371</v>
+      </c>
+      <c r="D10" s="28" t="s">
         <v>372</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="F10" s="28" t="s">
         <v>373</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>374</v>
       </c>
       <c r="H10" s="20"/>
       <c r="N10" s="33"/>
@@ -5955,16 +5940,16 @@
     </row>
     <row r="11" spans="1:34" s="29" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B11" s="29" t="s">
+        <v>374</v>
+      </c>
+      <c r="D11" s="29" t="s">
         <v>375</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="F11" s="19" t="s">
         <v>376</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>377</v>
       </c>
       <c r="N11" s="34"/>
       <c r="O11" s="45"/>
@@ -5977,17 +5962,17 @@
     </row>
     <row r="12" spans="1:34" s="28" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B12" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="D12" s="28" t="s">
         <v>378</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>379</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="28" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N12" s="33"/>
       <c r="O12" s="44"/>
@@ -6000,17 +5985,17 @@
     </row>
     <row r="13" spans="1:34" s="28" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B13" s="28" t="s">
+        <v>380</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>381</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>382</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="28" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N13" s="33"/>
       <c r="O13" s="44"/>
@@ -6023,60 +6008,60 @@
     </row>
     <row r="14" spans="1:34" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
+        <v>399</v>
+      </c>
+      <c r="B14" s="71" t="s">
+        <v>386</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>387</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" s="78" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
         <v>400</v>
       </c>
-      <c r="B14" s="89" t="s">
-        <v>387</v>
-      </c>
-      <c r="D14" s="19" t="s">
+      <c r="B15" s="79" t="s">
         <v>388</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" s="96" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="D15" s="77" t="s">
+        <v>389</v>
+      </c>
+      <c r="F15" s="79" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" s="78" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
         <v>401</v>
       </c>
-      <c r="B15" s="97" t="s">
-        <v>389</v>
-      </c>
-      <c r="D15" s="95" t="s">
-        <v>390</v>
-      </c>
-      <c r="F15" s="97" t="s">
+      <c r="B16" s="79" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="16" spans="1:34" s="96" customFormat="1" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>402</v>
-      </c>
-      <c r="B16" s="97" t="s">
+      <c r="D16" s="77" t="s">
         <v>392</v>
       </c>
-      <c r="D16" s="95" t="s">
+      <c r="F16" s="79" t="s">
         <v>393</v>
-      </c>
-      <c r="F16" s="97" t="s">
-        <v>394</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9:H13" xr:uid="{DB701270-40E2-411B-8007-12813316A915}">

</xml_diff>